<commit_message>
Fix getting fields of columns name that contains space
update test to run

refactor: split classes to reader & generator & writer

update test

add tests
</commit_message>
<xml_diff>
--- a/demo/mission.xlsx
+++ b/demo/mission.xlsx
@@ -1,32 +1,226 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4635"/>
+    <workbookView windowWidth="19095" windowHeight="10065"/>
   </bookViews>
   <sheets>
     <sheet name="Mission" sheetId="1" r:id="rId1"/>
     <sheet name="MissionLevel" sheetId="2" r:id="rId2"/>
     <sheet name="Reference" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>requirement_type</t>
+  </si>
+  <si>
+    <t>parameters</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>level required</t>
+  </si>
+  <si>
+    <t>Win x time any game</t>
+  </si>
+  <si>
+    <t>Win in any game</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Play x time with any game</t>
+  </si>
+  <si>
+    <t>Play in any game</t>
+  </si>
+  <si>
+    <t>Exchange gold</t>
+  </si>
+  <si>
+    <t>Exchange Gold from oncase x times with any game - any value accepted</t>
+  </si>
+  <si>
+    <t>Watch video ads</t>
+  </si>
+  <si>
+    <t>Watch videos ads x times with any game (Bixa, Holla, Xito, TienLen)</t>
+  </si>
+  <si>
+    <t>Level up</t>
+  </si>
+  <si>
+    <t>Reach to x level (10, 20, 30, 40, 50...)</t>
+  </si>
+  <si>
+    <t>Own gold</t>
+  </si>
+  <si>
+    <t>Own x amount of gold (1 mil, 5mil, 10 mil)</t>
+  </si>
+  <si>
+    <t>Channel STREET win</t>
+  </si>
+  <si>
+    <t>Win at channel STREET</t>
+  </si>
+  <si>
+    <t>Channel FREE win</t>
+  </si>
+  <si>
+    <t>Win at channel FREE</t>
+  </si>
+  <si>
+    <t>Channel AMATUER win</t>
+  </si>
+  <si>
+    <t>Win at channel AMATUER</t>
+  </si>
+  <si>
+    <t>Channel PRO win</t>
+  </si>
+  <si>
+    <t>Win at channel PRO</t>
+  </si>
+  <si>
+    <t>Channel OPEN win</t>
+  </si>
+  <si>
+    <t>Win at channel OPEN</t>
+  </si>
+  <si>
+    <t>Any channel win</t>
+  </si>
+  <si>
+    <t>Win at any channel</t>
+  </si>
+  <si>
+    <t>Sending gift</t>
+  </si>
+  <si>
+    <t>Sending gift to x friends (5, 10, 15, 20...)</t>
+  </si>
+  <si>
+    <t>Receiveing gift</t>
+  </si>
+  <si>
+    <t>Receiving gift from x friend (5, 10, 15, 20...)</t>
+  </si>
+  <si>
+    <t>Making friend</t>
+  </si>
+  <si>
+    <t>Making x friends (50, 100...)</t>
+  </si>
+  <si>
+    <t>Win 3 chi</t>
+  </si>
+  <si>
+    <t>Win 3 chi x competitor (5, 10, 15...)</t>
+  </si>
+  <si>
+    <t>Have Ace</t>
+  </si>
+  <si>
+    <t>Have Ace in x games</t>
+  </si>
+  <si>
+    <t>Mau Binh at x times (5, 10, 15...)</t>
+  </si>
+  <si>
+    <t>Holla Win 1st place</t>
+  </si>
+  <si>
+    <t>Win 1st place x times</t>
+  </si>
+  <si>
+    <t>Stolen card</t>
+  </si>
+  <si>
+    <t>Stolen card x times</t>
+  </si>
+  <si>
+    <t>Less than 10 pts</t>
+  </si>
+  <si>
+    <t>End the game with less than 10 points</t>
+  </si>
+  <si>
+    <t>Win 5 cards mode</t>
+  </si>
+  <si>
+    <t>Win x times in 5 cards mode</t>
+  </si>
+  <si>
+    <t>Win 7 cards mode</t>
+  </si>
+  <si>
+    <t>Win x times in 7 cards mode</t>
+  </si>
+  <si>
+    <t>All-in</t>
+  </si>
+  <si>
+    <t>All-in x time</t>
+  </si>
+  <si>
+    <t>Win game with 3 spade</t>
+  </si>
+  <si>
+    <t>Win the game with 3 spade (any game mode)</t>
+  </si>
+  <si>
+    <t>Booming</t>
+  </si>
+  <si>
+    <t>Booming x times (any game mode) - No need care about the game result</t>
+  </si>
+  <si>
+    <t>Win 1st place</t>
+  </si>
+  <si>
+    <t>mission_id</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>requirement_value</t>
+  </si>
+  <si>
+    <t>reward_gold</t>
+  </si>
   <si>
     <t>Mission requirement</t>
   </si>
@@ -37,204 +231,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>mission_id</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>params</t>
-  </si>
-  <si>
-    <t>requirement_value</t>
-  </si>
-  <si>
-    <t>reward_gold</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>frequency</t>
-  </si>
-  <si>
-    <t>requirement_type</t>
-  </si>
-  <si>
-    <t>parameters</t>
-  </si>
-  <si>
-    <t>Win x time any game</t>
-  </si>
-  <si>
-    <t>Win in any game</t>
-  </si>
-  <si>
-    <t>Play x time with any game</t>
-  </si>
-  <si>
-    <t>Play in any game</t>
-  </si>
-  <si>
-    <t>Exchange gold</t>
-  </si>
-  <si>
-    <t>Exchange Gold from oncase x times with any game - any value accepted</t>
-  </si>
-  <si>
-    <t>Watch video ads</t>
-  </si>
-  <si>
-    <t>Watch videos ads x times with any game (Bixa, Holla, Xito, TienLen)</t>
-  </si>
-  <si>
-    <t>Level up</t>
-  </si>
-  <si>
-    <t>Reach to x level (10, 20, 30, 40, 50...)</t>
-  </si>
-  <si>
-    <t>Own gold</t>
-  </si>
-  <si>
-    <t>Own x amount of gold (1 mil, 5mil, 10 mil)</t>
-  </si>
-  <si>
-    <t>Channel STREET win</t>
-  </si>
-  <si>
-    <t>Win at channel STREET</t>
-  </si>
-  <si>
-    <t>Channel FREE win</t>
-  </si>
-  <si>
-    <t>Win at channel FREE</t>
-  </si>
-  <si>
-    <t>Channel AMATUER win</t>
-  </si>
-  <si>
-    <t>Win at channel AMATUER</t>
-  </si>
-  <si>
-    <t>Channel PRO win</t>
-  </si>
-  <si>
-    <t>Win at channel PRO</t>
-  </si>
-  <si>
-    <t>Channel OPEN win</t>
-  </si>
-  <si>
-    <t>Win at channel OPEN</t>
-  </si>
-  <si>
-    <t>Any channel win</t>
-  </si>
-  <si>
-    <t>Win at any channel</t>
-  </si>
-  <si>
-    <t>Sending gift</t>
-  </si>
-  <si>
-    <t>Sending gift to x friends (5, 10, 15, 20...)</t>
-  </si>
-  <si>
-    <t>Receiveing gift</t>
-  </si>
-  <si>
-    <t>Receiving gift from x friend (5, 10, 15, 20...)</t>
-  </si>
-  <si>
-    <t>Making friend</t>
-  </si>
-  <si>
-    <t>Making x friends (50, 100...)</t>
-  </si>
-  <si>
-    <t>Win 3 chi</t>
-  </si>
-  <si>
-    <t>Win 3 chi x competitor (5, 10, 15...)</t>
-  </si>
-  <si>
-    <t>Have Ace</t>
-  </si>
-  <si>
-    <t>Have Ace in x games</t>
-  </si>
-  <si>
-    <t>Mau Binh at x times (5, 10, 15...)</t>
-  </si>
-  <si>
-    <t>Holla Win 1st place</t>
-  </si>
-  <si>
-    <t>Win 1st place x times</t>
-  </si>
-  <si>
-    <t>Stolen card</t>
-  </si>
-  <si>
-    <t>Stolen card x times</t>
-  </si>
-  <si>
-    <t>Less than 10 pts</t>
-  </si>
-  <si>
-    <t>End the game with less than 10 points</t>
-  </si>
-  <si>
-    <t>Win 5 cards mode</t>
-  </si>
-  <si>
-    <t>Win x times in 5 cards mode</t>
-  </si>
-  <si>
-    <t>Win 7 cards mode</t>
-  </si>
-  <si>
-    <t>Win x times in 7 cards mode</t>
-  </si>
-  <si>
-    <t>All-in</t>
-  </si>
-  <si>
-    <t>All-in x time</t>
-  </si>
-  <si>
-    <t>Win game with 3 spade</t>
-  </si>
-  <si>
-    <t>Win the game with 3 spade (any game mode)</t>
-  </si>
-  <si>
-    <t>Booming</t>
-  </si>
-  <si>
-    <t>Booming x times (any game mode) - No need care about the game result</t>
-  </si>
-  <si>
-    <t>Win 1st place</t>
-  </si>
-  <si>
     <t>WIN_IN_ANY_GAME</t>
   </si>
   <si>
@@ -314,33 +310,366 @@
   </si>
   <si>
     <t>TIENLEN_WIN_FIRST_PLACE</t>
-  </si>
-  <si>
-    <t>active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -348,24 +677,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -414,7 +1029,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,7 +1064,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,70 +1238,69 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="66.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="13.8571428571429" customWidth="1"/>
+    <col min="7" max="7" width="17.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="11.1428571428571" customWidth="1"/>
+    <col min="10" max="10" width="14.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -701,21 +1315,24 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -730,21 +1347,24 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -759,21 +1379,24 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -788,21 +1411,24 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -817,21 +1443,24 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -846,21 +1475,24 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -875,21 +1507,24 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -904,21 +1539,24 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9">
         <v>8</v>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -933,21 +1571,24 @@
         <v>9</v>
       </c>
       <c r="H10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -962,21 +1603,24 @@
         <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -991,21 +1635,24 @@
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1020,21 +1667,24 @@
         <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1049,21 +1699,24 @@
         <v>13</v>
       </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1078,21 +1731,24 @@
         <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1107,21 +1763,24 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -1136,21 +1795,24 @@
         <v>16</v>
       </c>
       <c r="H17" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1165,21 +1827,24 @@
         <v>17</v>
       </c>
       <c r="H18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1194,21 +1859,24 @@
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -1223,21 +1891,24 @@
         <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1252,21 +1923,24 @@
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1281,21 +1955,24 @@
         <v>21</v>
       </c>
       <c r="H22" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1310,21 +1987,24 @@
         <v>22</v>
       </c>
       <c r="H23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D24">
         <v>3</v>
@@ -1339,21 +2019,24 @@
         <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1368,21 +2051,24 @@
         <v>24</v>
       </c>
       <c r="H25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -1397,21 +2083,24 @@
         <v>25</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D27">
         <v>3</v>
@@ -1426,21 +2115,24 @@
         <v>26</v>
       </c>
       <c r="H27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1455,49 +2147,54 @@
         <v>27</v>
       </c>
       <c r="H28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
       </c>
+      <c r="J28">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="18.4285714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1505,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -1514,7 +2211,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1522,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1531,7 +2228,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1539,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -1548,7 +2245,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1556,7 +2253,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -1565,7 +2262,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1573,7 +2270,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1582,7 +2279,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1590,7 +2287,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1599,7 +2296,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1607,7 +2304,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1616,7 +2313,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1624,7 +2321,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1633,7 +2330,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1641,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -1650,7 +2347,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1658,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D11">
         <v>1000</v>
@@ -1667,7 +2364,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1675,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <f>D11+500</f>
@@ -1685,7 +2382,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1693,7 +2390,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D13">
         <f>D12+500</f>
@@ -1703,7 +2400,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1711,7 +2408,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <f>D13+500</f>
@@ -1721,7 +2418,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1729,7 +2426,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D15">
         <f>D14+500</f>
@@ -1739,7 +2436,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1747,7 +2444,7 @@
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1756,7 +2453,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>7</v>
       </c>
@@ -1764,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1773,7 +2470,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>7</v>
       </c>
@@ -1781,7 +2478,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1790,7 +2487,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>7</v>
       </c>
@@ -1798,7 +2495,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1807,7 +2504,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1815,7 +2512,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D20">
         <v>5</v>
@@ -1824,7 +2521,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1832,7 +2529,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1841,7 +2538,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>8</v>
       </c>
@@ -1849,7 +2546,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1858,7 +2555,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1866,7 +2563,7 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1875,7 +2572,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>8</v>
       </c>
@@ -1883,7 +2580,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1892,7 +2589,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1900,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D25">
         <v>5</v>
@@ -1909,7 +2606,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>9</v>
       </c>
@@ -1917,7 +2614,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -1926,7 +2623,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1934,7 +2631,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -1943,7 +2640,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1951,7 +2648,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1960,7 +2657,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1968,7 +2665,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -1977,7 +2674,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1985,7 +2682,7 @@
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D30">
         <v>5</v>
@@ -1994,7 +2691,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>10</v>
       </c>
@@ -2002,7 +2699,7 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -2011,7 +2708,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>10</v>
       </c>
@@ -2019,7 +2716,7 @@
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -2028,7 +2725,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>10</v>
       </c>
@@ -2036,7 +2733,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -2045,7 +2742,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>10</v>
       </c>
@@ -2053,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -2062,7 +2759,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>10</v>
       </c>
@@ -2070,7 +2767,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>5</v>
@@ -2079,7 +2776,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>11</v>
       </c>
@@ -2087,7 +2784,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <v>1</v>
@@ -2096,7 +2793,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>11</v>
       </c>
@@ -2104,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -2113,7 +2810,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>11</v>
       </c>
@@ -2121,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -2130,7 +2827,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>11</v>
       </c>
@@ -2138,7 +2835,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -2147,7 +2844,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>11</v>
       </c>
@@ -2155,7 +2852,7 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <v>5</v>
@@ -2164,7 +2861,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>12</v>
       </c>
@@ -2172,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -2181,7 +2878,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>12</v>
       </c>
@@ -2189,7 +2886,7 @@
         <v>2</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -2198,7 +2895,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>12</v>
       </c>
@@ -2206,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <v>3</v>
@@ -2215,7 +2912,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>12</v>
       </c>
@@ -2223,7 +2920,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D44">
         <v>4</v>
@@ -2232,7 +2929,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>12</v>
       </c>
@@ -2240,7 +2937,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D45">
         <v>5</v>
@@ -2249,7 +2946,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>13</v>
       </c>
@@ -2257,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -2266,7 +2963,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>13</v>
       </c>
@@ -2274,7 +2971,7 @@
         <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D47">
         <v>2</v>
@@ -2283,7 +2980,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>13</v>
       </c>
@@ -2291,7 +2988,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D48">
         <v>3</v>
@@ -2300,7 +2997,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>13</v>
       </c>
@@ -2308,7 +3005,7 @@
         <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D49">
         <v>4</v>
@@ -2317,7 +3014,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>13</v>
       </c>
@@ -2325,7 +3022,7 @@
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D50">
         <v>5</v>
@@ -2334,7 +3031,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>14</v>
       </c>
@@ -2342,7 +3039,7 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D51">
         <v>1</v>
@@ -2351,7 +3048,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>14</v>
       </c>
@@ -2359,7 +3056,7 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D52">
         <v>2</v>
@@ -2368,7 +3065,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>14</v>
       </c>
@@ -2376,7 +3073,7 @@
         <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D53">
         <v>3</v>
@@ -2385,7 +3082,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>14</v>
       </c>
@@ -2393,7 +3090,7 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>4</v>
@@ -2402,7 +3099,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>14</v>
       </c>
@@ -2410,7 +3107,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D55">
         <v>5</v>
@@ -2419,7 +3116,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>15</v>
       </c>
@@ -2427,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -2436,7 +3133,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>15</v>
       </c>
@@ -2444,7 +3141,7 @@
         <v>2</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -2453,7 +3150,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>15</v>
       </c>
@@ -2461,7 +3158,7 @@
         <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>3</v>
@@ -2470,7 +3167,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>15</v>
       </c>
@@ -2478,7 +3175,7 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -2487,7 +3184,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>15</v>
       </c>
@@ -2495,7 +3192,7 @@
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D60">
         <v>5</v>
@@ -2504,7 +3201,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>16</v>
       </c>
@@ -2512,7 +3209,7 @@
         <v>1</v>
       </c>
       <c r="C61" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D61">
         <v>3</v>
@@ -2521,7 +3218,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>17</v>
       </c>
@@ -2529,7 +3226,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D62">
         <v>3</v>
@@ -2538,7 +3235,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>18</v>
       </c>
@@ -2546,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D63">
         <v>3</v>
@@ -2555,7 +3252,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>19</v>
       </c>
@@ -2563,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D64">
         <v>3</v>
@@ -2572,7 +3269,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>20</v>
       </c>
@@ -2580,7 +3277,7 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D65">
         <v>3</v>
@@ -2589,7 +3286,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>21</v>
       </c>
@@ -2597,7 +3294,7 @@
         <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D66">
         <v>3</v>
@@ -2606,7 +3303,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>22</v>
       </c>
@@ -2614,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D67">
         <v>3</v>
@@ -2623,7 +3320,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>23</v>
       </c>
@@ -2631,7 +3328,7 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>3</v>
@@ -2640,7 +3337,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>24</v>
       </c>
@@ -2648,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D69">
         <v>3</v>
@@ -2657,7 +3354,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>25</v>
       </c>
@@ -2665,7 +3362,7 @@
         <v>1</v>
       </c>
       <c r="C70" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D70">
         <v>3</v>
@@ -2674,7 +3371,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>26</v>
       </c>
@@ -2682,7 +3379,7 @@
         <v>1</v>
       </c>
       <c r="C71" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D71">
         <v>3</v>
@@ -2691,7 +3388,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>27</v>
       </c>
@@ -2699,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="C72" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D72">
         <v>3</v>
@@ -2709,253 +3406,256 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B23">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B24">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B25">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B26">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B29">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>